<commit_message>
growth data script and figures added
</commit_message>
<xml_diff>
--- a/data/growth/growth.xlsx
+++ b/data/growth/growth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinebaird/Desktop/GitHub/polyIC-larvae/data/growth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168A14A9-1139-6A4B-A82C-648DE1334591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4352B040-331D-A545-8356-2CD49D005E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="500" windowWidth="17540" windowHeight="15840" xr2:uid="{BA24E048-5078-7B4D-9000-CCF0539A485F}"/>
+    <workbookView xWindow="12100" yWindow="500" windowWidth="17540" windowHeight="15840" xr2:uid="{BA24E048-5078-7B4D-9000-CCF0539A485F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB36B54-B7B4-0742-A47F-176219A7FAF5}">
   <dimension ref="A1:G1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I972" sqref="I972"/>
+    <sheetView tabSelected="1" topLeftCell="A853" workbookViewId="0">
+      <selection activeCell="E861" sqref="E861"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17711,7 +17711,7 @@
         <v>59</v>
       </c>
       <c r="E861">
-        <v>45</v>
+        <v>4.5</v>
       </c>
       <c r="F861" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
added more growth data to datasheet
</commit_message>
<xml_diff>
--- a/data/growth/growth.xlsx
+++ b/data/growth/growth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinebaird/Desktop/GitHub/polyIC-larvae/data/growth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4352B040-331D-A545-8356-2CD49D005E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99263076-505D-354E-AED1-696B3FD83F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12100" yWindow="500" windowWidth="17540" windowHeight="15840" xr2:uid="{BA24E048-5078-7B4D-9000-CCF0539A485F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17540" windowHeight="15840" xr2:uid="{BA24E048-5078-7B4D-9000-CCF0539A485F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3011" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3611" uniqueCount="23">
   <si>
     <t>control</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>20250206_treated5_size.jpeg</t>
+  </si>
+  <si>
+    <t>control_20250530.jpeg</t>
+  </si>
+  <si>
+    <t>treated_20250530.jpeg</t>
   </si>
 </sst>
 </file>
@@ -480,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB36B54-B7B4-0742-A47F-176219A7FAF5}">
-  <dimension ref="A1:G1002"/>
+  <dimension ref="A1:G1202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A853" workbookViewId="0">
-      <selection activeCell="E861" sqref="E861"/>
+    <sheetView tabSelected="1" topLeftCell="A1174" workbookViewId="0">
+      <selection activeCell="E1206" sqref="E1206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20537,6 +20543,4006 @@
         <v>20</v>
       </c>
     </row>
+    <row r="1003" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1003">
+        <v>20250530</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1003">
+        <v>1</v>
+      </c>
+      <c r="E1003">
+        <v>11.17</v>
+      </c>
+      <c r="F1003" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1004">
+        <v>20250530</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1004">
+        <v>2</v>
+      </c>
+      <c r="E1004">
+        <v>7.39</v>
+      </c>
+      <c r="F1004" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1005">
+        <v>20250530</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1005">
+        <v>3</v>
+      </c>
+      <c r="E1005">
+        <v>7.91</v>
+      </c>
+      <c r="F1005" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1006">
+        <v>20250530</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1006">
+        <v>4</v>
+      </c>
+      <c r="E1006">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="F1006" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1007">
+        <v>20250530</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1007">
+        <v>5</v>
+      </c>
+      <c r="E1007">
+        <v>9.34</v>
+      </c>
+      <c r="F1007" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1008">
+        <v>20250530</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1008">
+        <v>6</v>
+      </c>
+      <c r="E1008">
+        <v>10.56</v>
+      </c>
+      <c r="F1008" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1009">
+        <v>20250530</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1009">
+        <v>7</v>
+      </c>
+      <c r="E1009">
+        <v>9.43</v>
+      </c>
+      <c r="F1009" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1010">
+        <v>20250530</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1010">
+        <v>8</v>
+      </c>
+      <c r="E1010">
+        <v>8.75</v>
+      </c>
+      <c r="F1010" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1011">
+        <v>20250530</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1011">
+        <v>9</v>
+      </c>
+      <c r="E1011">
+        <v>7.82</v>
+      </c>
+      <c r="F1011" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1012">
+        <v>20250530</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1012">
+        <v>10</v>
+      </c>
+      <c r="E1012">
+        <v>9.08</v>
+      </c>
+      <c r="F1012" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1013">
+        <v>20250530</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1013">
+        <v>11</v>
+      </c>
+      <c r="E1013">
+        <v>7.72</v>
+      </c>
+      <c r="F1013" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1014">
+        <v>20250530</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1014">
+        <v>12</v>
+      </c>
+      <c r="E1014">
+        <v>7.55</v>
+      </c>
+      <c r="F1014" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1015">
+        <v>20250530</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1015">
+        <v>13</v>
+      </c>
+      <c r="E1015">
+        <v>10.17</v>
+      </c>
+      <c r="F1015" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1016">
+        <v>20250530</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1016">
+        <v>14</v>
+      </c>
+      <c r="E1016">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="F1016" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1017">
+        <v>20250530</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1017">
+        <v>15</v>
+      </c>
+      <c r="E1017">
+        <v>10.44</v>
+      </c>
+      <c r="F1017" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1018">
+        <v>20250530</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1018">
+        <v>16</v>
+      </c>
+      <c r="E1018">
+        <v>6.54</v>
+      </c>
+      <c r="F1018" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1019">
+        <v>20250530</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1019">
+        <v>17</v>
+      </c>
+      <c r="E1019">
+        <v>10.93</v>
+      </c>
+      <c r="F1019" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1020">
+        <v>20250530</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1020">
+        <v>18</v>
+      </c>
+      <c r="E1020">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="F1020" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1021">
+        <v>20250530</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1021">
+        <v>19</v>
+      </c>
+      <c r="E1021">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="F1021" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1022">
+        <v>20250530</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1022">
+        <v>20</v>
+      </c>
+      <c r="E1022">
+        <v>8.06</v>
+      </c>
+      <c r="F1022" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1023">
+        <v>20250530</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1023">
+        <v>21</v>
+      </c>
+      <c r="E1023">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="F1023" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1024">
+        <v>20250530</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1024">
+        <v>22</v>
+      </c>
+      <c r="E1024">
+        <v>5.45</v>
+      </c>
+      <c r="F1024" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1025">
+        <v>20250530</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1025">
+        <v>23</v>
+      </c>
+      <c r="E1025">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="F1025" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1026">
+        <v>20250530</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1026">
+        <v>24</v>
+      </c>
+      <c r="E1026">
+        <v>7.87</v>
+      </c>
+      <c r="F1026" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1027">
+        <v>20250530</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1027">
+        <v>25</v>
+      </c>
+      <c r="E1027">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="F1027" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1028">
+        <v>20250530</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1028">
+        <v>26</v>
+      </c>
+      <c r="E1028">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="F1028" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1029">
+        <v>20250530</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1029">
+        <v>27</v>
+      </c>
+      <c r="E1029">
+        <v>7.5</v>
+      </c>
+      <c r="F1029" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1030">
+        <v>20250530</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1030">
+        <v>28</v>
+      </c>
+      <c r="E1030">
+        <v>7.8</v>
+      </c>
+      <c r="F1030" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1031">
+        <v>20250530</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1031">
+        <v>29</v>
+      </c>
+      <c r="E1031">
+        <v>7.86</v>
+      </c>
+      <c r="F1031" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1032">
+        <v>20250530</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1032">
+        <v>30</v>
+      </c>
+      <c r="E1032">
+        <v>9.08</v>
+      </c>
+      <c r="F1032" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1033">
+        <v>20250530</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1033">
+        <v>31</v>
+      </c>
+      <c r="E1033">
+        <v>12.55</v>
+      </c>
+      <c r="F1033" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1034">
+        <v>20250530</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1034">
+        <v>32</v>
+      </c>
+      <c r="E1034">
+        <v>9.18</v>
+      </c>
+      <c r="F1034" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1035">
+        <v>20250530</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1035">
+        <v>33</v>
+      </c>
+      <c r="E1035">
+        <v>8.06</v>
+      </c>
+      <c r="F1035" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1036">
+        <v>20250530</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1036" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1036">
+        <v>34</v>
+      </c>
+      <c r="E1036">
+        <v>11.04</v>
+      </c>
+      <c r="F1036" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1037">
+        <v>20250530</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1037" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1037">
+        <v>35</v>
+      </c>
+      <c r="E1037">
+        <v>8.1</v>
+      </c>
+      <c r="F1037" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1038">
+        <v>20250530</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1038">
+        <v>36</v>
+      </c>
+      <c r="E1038">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="F1038" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1039">
+        <v>20250530</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1039">
+        <v>37</v>
+      </c>
+      <c r="E1039">
+        <v>11.15</v>
+      </c>
+      <c r="F1039" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1040">
+        <v>20250530</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1040">
+        <v>38</v>
+      </c>
+      <c r="E1040">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="F1040" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1041">
+        <v>20250530</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1041" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1041">
+        <v>39</v>
+      </c>
+      <c r="E1041">
+        <v>12.14</v>
+      </c>
+      <c r="F1041" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1042">
+        <v>20250530</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1042" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1042">
+        <v>40</v>
+      </c>
+      <c r="E1042">
+        <v>6.66</v>
+      </c>
+      <c r="F1042" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1043">
+        <v>20250530</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1043" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1043">
+        <v>41</v>
+      </c>
+      <c r="E1043">
+        <v>9.08</v>
+      </c>
+      <c r="F1043" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1044">
+        <v>20250530</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1044" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1044">
+        <v>42</v>
+      </c>
+      <c r="E1044">
+        <v>10.48</v>
+      </c>
+      <c r="F1044" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1045">
+        <v>20250530</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1045" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1045">
+        <v>43</v>
+      </c>
+      <c r="E1045">
+        <v>8.06</v>
+      </c>
+      <c r="F1045" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1046">
+        <v>20250530</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1046">
+        <v>44</v>
+      </c>
+      <c r="E1046">
+        <v>9.5</v>
+      </c>
+      <c r="F1046" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1047">
+        <v>20250530</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1047">
+        <v>45</v>
+      </c>
+      <c r="E1047">
+        <v>7.82</v>
+      </c>
+      <c r="F1047" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1048">
+        <v>20250530</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1048" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1048">
+        <v>46</v>
+      </c>
+      <c r="E1048">
+        <v>7.64</v>
+      </c>
+      <c r="F1048" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1049">
+        <v>20250530</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1049" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1049">
+        <v>47</v>
+      </c>
+      <c r="E1049">
+        <v>10.15</v>
+      </c>
+      <c r="F1049" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1050">
+        <v>20250530</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1050" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1050">
+        <v>48</v>
+      </c>
+      <c r="E1050">
+        <v>6.67</v>
+      </c>
+      <c r="F1050" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1051">
+        <v>20250530</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1051" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1051">
+        <v>49</v>
+      </c>
+      <c r="E1051">
+        <v>12.3</v>
+      </c>
+      <c r="F1051" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1052">
+        <v>20250530</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1052" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1052">
+        <v>50</v>
+      </c>
+      <c r="E1052">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="F1052" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1053">
+        <v>20250530</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1053" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1053">
+        <v>51</v>
+      </c>
+      <c r="E1053">
+        <v>8.11</v>
+      </c>
+      <c r="F1053" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1054">
+        <v>20250530</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1054" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1054">
+        <v>52</v>
+      </c>
+      <c r="E1054">
+        <v>11.55</v>
+      </c>
+      <c r="F1054" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1055">
+        <v>20250530</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1055" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1055">
+        <v>53</v>
+      </c>
+      <c r="E1055">
+        <v>11.74</v>
+      </c>
+      <c r="F1055" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1056">
+        <v>20250530</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1056" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1056">
+        <v>54</v>
+      </c>
+      <c r="E1056">
+        <v>10.42</v>
+      </c>
+      <c r="F1056" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1057">
+        <v>20250530</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1057" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1057">
+        <v>55</v>
+      </c>
+      <c r="E1057">
+        <v>8.68</v>
+      </c>
+      <c r="F1057" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1058">
+        <v>20250530</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1058" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1058">
+        <v>56</v>
+      </c>
+      <c r="E1058">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="F1058" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1059">
+        <v>20250530</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1059">
+        <v>57</v>
+      </c>
+      <c r="E1059">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="F1059" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1060">
+        <v>20250530</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1060" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1060">
+        <v>58</v>
+      </c>
+      <c r="E1060">
+        <v>7.53</v>
+      </c>
+      <c r="F1060" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1061">
+        <v>20250530</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1061" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1061">
+        <v>59</v>
+      </c>
+      <c r="E1061">
+        <v>10.19</v>
+      </c>
+      <c r="F1061" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1062">
+        <v>20250530</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1062">
+        <v>60</v>
+      </c>
+      <c r="E1062">
+        <v>8.6</v>
+      </c>
+      <c r="F1062" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1063">
+        <v>20250530</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1063">
+        <v>61</v>
+      </c>
+      <c r="E1063">
+        <v>8.98</v>
+      </c>
+      <c r="F1063" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1064">
+        <v>20250530</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1064" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1064">
+        <v>62</v>
+      </c>
+      <c r="E1064">
+        <v>7.5</v>
+      </c>
+      <c r="F1064" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1065">
+        <v>20250530</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1065" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1065">
+        <v>63</v>
+      </c>
+      <c r="E1065">
+        <v>10.34</v>
+      </c>
+      <c r="F1065" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1066">
+        <v>20250530</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1066" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1066">
+        <v>64</v>
+      </c>
+      <c r="E1066">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="F1066" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1067">
+        <v>20250530</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1067" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1067">
+        <v>65</v>
+      </c>
+      <c r="E1067">
+        <v>8.01</v>
+      </c>
+      <c r="F1067" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1068">
+        <v>20250530</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1068" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1068">
+        <v>66</v>
+      </c>
+      <c r="E1068">
+        <v>10.32</v>
+      </c>
+      <c r="F1068" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1069">
+        <v>20250530</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1069" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1069">
+        <v>67</v>
+      </c>
+      <c r="E1069">
+        <v>10.46</v>
+      </c>
+      <c r="F1069" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1070">
+        <v>20250530</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1070" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1070">
+        <v>68</v>
+      </c>
+      <c r="E1070">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="F1070" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1071">
+        <v>20250530</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1071" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1071">
+        <v>69</v>
+      </c>
+      <c r="E1071">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="F1071" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1072">
+        <v>20250530</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1072" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1072">
+        <v>70</v>
+      </c>
+      <c r="E1072">
+        <v>8.85</v>
+      </c>
+      <c r="F1072" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1073">
+        <v>20250530</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1073" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1073">
+        <v>71</v>
+      </c>
+      <c r="E1073">
+        <v>10.32</v>
+      </c>
+      <c r="F1073" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1074">
+        <v>20250530</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1074" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1074">
+        <v>72</v>
+      </c>
+      <c r="E1074">
+        <v>7.7</v>
+      </c>
+      <c r="F1074" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1075">
+        <v>20250530</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1075" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1075">
+        <v>73</v>
+      </c>
+      <c r="E1075">
+        <v>11</v>
+      </c>
+      <c r="F1075" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1076">
+        <v>20250530</v>
+      </c>
+      <c r="B1076" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1076" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1076">
+        <v>74</v>
+      </c>
+      <c r="E1076">
+        <v>8.33</v>
+      </c>
+      <c r="F1076" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1077">
+        <v>20250530</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1077" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1077">
+        <v>75</v>
+      </c>
+      <c r="E1077">
+        <v>6.45</v>
+      </c>
+      <c r="F1077" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1078">
+        <v>20250530</v>
+      </c>
+      <c r="B1078" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1078" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1078">
+        <v>76</v>
+      </c>
+      <c r="E1078">
+        <v>9.56</v>
+      </c>
+      <c r="F1078" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1079">
+        <v>20250530</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1079" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1079">
+        <v>77</v>
+      </c>
+      <c r="E1079">
+        <v>8.58</v>
+      </c>
+      <c r="F1079" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1080">
+        <v>20250530</v>
+      </c>
+      <c r="B1080" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1080" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1080">
+        <v>78</v>
+      </c>
+      <c r="E1080">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="F1080" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1081">
+        <v>20250530</v>
+      </c>
+      <c r="B1081" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1081" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1081">
+        <v>79</v>
+      </c>
+      <c r="E1081">
+        <v>9.09</v>
+      </c>
+      <c r="F1081" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1082">
+        <v>20250530</v>
+      </c>
+      <c r="B1082" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1082" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1082">
+        <v>80</v>
+      </c>
+      <c r="E1082">
+        <v>9.82</v>
+      </c>
+      <c r="F1082" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1083">
+        <v>20250530</v>
+      </c>
+      <c r="B1083" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1083" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1083">
+        <v>81</v>
+      </c>
+      <c r="E1083">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="F1083" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1084">
+        <v>20250530</v>
+      </c>
+      <c r="B1084" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1084" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1084">
+        <v>82</v>
+      </c>
+      <c r="E1084">
+        <v>10.82</v>
+      </c>
+      <c r="F1084" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1085">
+        <v>20250530</v>
+      </c>
+      <c r="B1085" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1085" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1085">
+        <v>83</v>
+      </c>
+      <c r="E1085">
+        <v>8.5</v>
+      </c>
+      <c r="F1085" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1086">
+        <v>20250530</v>
+      </c>
+      <c r="B1086" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1086" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1086">
+        <v>84</v>
+      </c>
+      <c r="E1086">
+        <v>7.18</v>
+      </c>
+      <c r="F1086" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1087">
+        <v>20250530</v>
+      </c>
+      <c r="B1087" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1087" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1087">
+        <v>85</v>
+      </c>
+      <c r="E1087">
+        <v>11.79</v>
+      </c>
+      <c r="F1087" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1088">
+        <v>20250530</v>
+      </c>
+      <c r="B1088" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1088" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1088">
+        <v>86</v>
+      </c>
+      <c r="E1088">
+        <v>8.34</v>
+      </c>
+      <c r="F1088" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1089">
+        <v>20250530</v>
+      </c>
+      <c r="B1089" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1089" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1089">
+        <v>87</v>
+      </c>
+      <c r="E1089">
+        <v>8.92</v>
+      </c>
+      <c r="F1089" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1090">
+        <v>20250530</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1090" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1090">
+        <v>88</v>
+      </c>
+      <c r="E1090">
+        <v>9.7360000000000007</v>
+      </c>
+      <c r="F1090" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1091">
+        <v>20250530</v>
+      </c>
+      <c r="B1091" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1091" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1091">
+        <v>89</v>
+      </c>
+      <c r="E1091">
+        <v>9.4469999999999992</v>
+      </c>
+      <c r="F1091" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1092">
+        <v>20250530</v>
+      </c>
+      <c r="B1092" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1092" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1092">
+        <v>90</v>
+      </c>
+      <c r="E1092">
+        <v>7.02</v>
+      </c>
+      <c r="F1092" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1093">
+        <v>20250530</v>
+      </c>
+      <c r="B1093" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1093" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1093">
+        <v>91</v>
+      </c>
+      <c r="E1093">
+        <v>11.44</v>
+      </c>
+      <c r="F1093" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1094">
+        <v>20250530</v>
+      </c>
+      <c r="B1094" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1094" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1094">
+        <v>92</v>
+      </c>
+      <c r="E1094">
+        <v>9.94</v>
+      </c>
+      <c r="F1094" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1095">
+        <v>20250530</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1095">
+        <v>93</v>
+      </c>
+      <c r="E1095">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="F1095" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1096">
+        <v>20250530</v>
+      </c>
+      <c r="B1096" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1096" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1096">
+        <v>94</v>
+      </c>
+      <c r="E1096">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="F1096" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1097">
+        <v>20250530</v>
+      </c>
+      <c r="B1097" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1097" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1097">
+        <v>95</v>
+      </c>
+      <c r="E1097">
+        <v>10.76</v>
+      </c>
+      <c r="F1097" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1098">
+        <v>20250530</v>
+      </c>
+      <c r="B1098" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1098" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1098">
+        <v>96</v>
+      </c>
+      <c r="E1098">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="F1098" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1099">
+        <v>20250530</v>
+      </c>
+      <c r="B1099" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1099" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1099">
+        <v>97</v>
+      </c>
+      <c r="E1099">
+        <v>8.89</v>
+      </c>
+      <c r="F1099" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1100">
+        <v>20250530</v>
+      </c>
+      <c r="B1100" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1100" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1100">
+        <v>98</v>
+      </c>
+      <c r="E1100">
+        <v>10.25</v>
+      </c>
+      <c r="F1100" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1101">
+        <v>20250530</v>
+      </c>
+      <c r="B1101" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1101" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1101">
+        <v>99</v>
+      </c>
+      <c r="E1101">
+        <v>9.81</v>
+      </c>
+      <c r="F1101" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1102">
+        <v>20250530</v>
+      </c>
+      <c r="B1102" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1102" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1102">
+        <v>100</v>
+      </c>
+      <c r="E1102">
+        <v>7.91</v>
+      </c>
+      <c r="F1102" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1103">
+        <v>20250530</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1103">
+        <v>1</v>
+      </c>
+      <c r="E1103">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="F1103" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1104">
+        <v>20250530</v>
+      </c>
+      <c r="B1104" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1104" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1104">
+        <v>2</v>
+      </c>
+      <c r="E1104">
+        <v>11.45</v>
+      </c>
+      <c r="F1104" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1105">
+        <v>20250530</v>
+      </c>
+      <c r="B1105" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1105" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1105">
+        <v>3</v>
+      </c>
+      <c r="E1105">
+        <v>11.63</v>
+      </c>
+      <c r="F1105" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1106">
+        <v>20250530</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1106">
+        <v>4</v>
+      </c>
+      <c r="E1106">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="F1106" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1107">
+        <v>20250530</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1107">
+        <v>5</v>
+      </c>
+      <c r="E1107">
+        <v>9.86</v>
+      </c>
+      <c r="F1107" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1108">
+        <v>20250530</v>
+      </c>
+      <c r="B1108" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1108" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1108">
+        <v>6</v>
+      </c>
+      <c r="E1108">
+        <v>8.48</v>
+      </c>
+      <c r="F1108" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1109">
+        <v>20250530</v>
+      </c>
+      <c r="B1109" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1109" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1109">
+        <v>7</v>
+      </c>
+      <c r="E1109">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F1109" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1110">
+        <v>20250530</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1110">
+        <v>8</v>
+      </c>
+      <c r="E1110">
+        <v>7.74</v>
+      </c>
+      <c r="F1110" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1111">
+        <v>20250530</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1111" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1111">
+        <v>9</v>
+      </c>
+      <c r="E1111">
+        <v>11.23</v>
+      </c>
+      <c r="F1111" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1112">
+        <v>20250530</v>
+      </c>
+      <c r="B1112" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1112" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1112">
+        <v>10</v>
+      </c>
+      <c r="E1112">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="F1112" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1113">
+        <v>20250530</v>
+      </c>
+      <c r="B1113" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1113" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1113">
+        <v>11</v>
+      </c>
+      <c r="E1113">
+        <v>9.48</v>
+      </c>
+      <c r="F1113" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1114">
+        <v>20250530</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1114" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1114">
+        <v>12</v>
+      </c>
+      <c r="E1114">
+        <v>9.48</v>
+      </c>
+      <c r="F1114" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1115">
+        <v>20250530</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1115" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1115">
+        <v>13</v>
+      </c>
+      <c r="E1115">
+        <v>7.59</v>
+      </c>
+      <c r="F1115" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1116">
+        <v>20250530</v>
+      </c>
+      <c r="B1116" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1116" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1116">
+        <v>14</v>
+      </c>
+      <c r="E1116">
+        <v>9.94</v>
+      </c>
+      <c r="F1116" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1117">
+        <v>20250530</v>
+      </c>
+      <c r="B1117" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1117" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1117">
+        <v>15</v>
+      </c>
+      <c r="E1117">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F1117" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1118">
+        <v>20250530</v>
+      </c>
+      <c r="B1118" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1118" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1118">
+        <v>16</v>
+      </c>
+      <c r="E1118">
+        <v>10.02</v>
+      </c>
+      <c r="F1118" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1119">
+        <v>20250530</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1119" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1119">
+        <v>17</v>
+      </c>
+      <c r="E1119">
+        <v>7.41</v>
+      </c>
+      <c r="F1119" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1120">
+        <v>20250530</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1120" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1120">
+        <v>18</v>
+      </c>
+      <c r="E1120">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F1120" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1121">
+        <v>20250530</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1121" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1121">
+        <v>19</v>
+      </c>
+      <c r="E1121">
+        <v>11.87</v>
+      </c>
+      <c r="F1121" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1122">
+        <v>20250530</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1122" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1122">
+        <v>20</v>
+      </c>
+      <c r="E1122">
+        <v>8.34</v>
+      </c>
+      <c r="F1122" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1123">
+        <v>20250530</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1123" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1123">
+        <v>21</v>
+      </c>
+      <c r="E1123">
+        <v>8.86</v>
+      </c>
+      <c r="F1123" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1124">
+        <v>20250530</v>
+      </c>
+      <c r="B1124" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1124" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1124">
+        <v>22</v>
+      </c>
+      <c r="E1124">
+        <v>11.2</v>
+      </c>
+      <c r="F1124" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1125">
+        <v>20250530</v>
+      </c>
+      <c r="B1125" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1125" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1125">
+        <v>23</v>
+      </c>
+      <c r="E1125">
+        <v>9.83</v>
+      </c>
+      <c r="F1125" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1126">
+        <v>20250530</v>
+      </c>
+      <c r="B1126" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1126" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1126">
+        <v>24</v>
+      </c>
+      <c r="E1126">
+        <v>10.91</v>
+      </c>
+      <c r="F1126" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1127">
+        <v>20250530</v>
+      </c>
+      <c r="B1127" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1127" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1127">
+        <v>25</v>
+      </c>
+      <c r="E1127">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="F1127" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1128">
+        <v>20250530</v>
+      </c>
+      <c r="B1128" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1128" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1128">
+        <v>26</v>
+      </c>
+      <c r="E1128">
+        <v>7.59</v>
+      </c>
+      <c r="F1128" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1129">
+        <v>20250530</v>
+      </c>
+      <c r="B1129" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1129" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1129">
+        <v>27</v>
+      </c>
+      <c r="E1129">
+        <v>7.93</v>
+      </c>
+      <c r="F1129" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1130">
+        <v>20250530</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1130" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1130">
+        <v>28</v>
+      </c>
+      <c r="E1130">
+        <v>9.07</v>
+      </c>
+      <c r="F1130" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1131">
+        <v>20250530</v>
+      </c>
+      <c r="B1131" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1131" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1131">
+        <v>29</v>
+      </c>
+      <c r="E1131">
+        <v>9.92</v>
+      </c>
+      <c r="F1131" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1132">
+        <v>20250530</v>
+      </c>
+      <c r="B1132" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1132" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1132">
+        <v>30</v>
+      </c>
+      <c r="E1132">
+        <v>9.31</v>
+      </c>
+      <c r="F1132" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1133">
+        <v>20250530</v>
+      </c>
+      <c r="B1133" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1133" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1133">
+        <v>31</v>
+      </c>
+      <c r="E1133">
+        <v>8.34</v>
+      </c>
+      <c r="F1133" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1134">
+        <v>20250530</v>
+      </c>
+      <c r="B1134" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1134" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1134">
+        <v>32</v>
+      </c>
+      <c r="E1134">
+        <v>8.7899999999999991</v>
+      </c>
+      <c r="F1134" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1135">
+        <v>20250530</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1135" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1135">
+        <v>33</v>
+      </c>
+      <c r="E1135">
+        <v>11.02</v>
+      </c>
+      <c r="F1135" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1136">
+        <v>20250530</v>
+      </c>
+      <c r="B1136" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1136" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1136">
+        <v>34</v>
+      </c>
+      <c r="E1136">
+        <v>10.82</v>
+      </c>
+      <c r="F1136" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1137">
+        <v>20250530</v>
+      </c>
+      <c r="B1137" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1137" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1137">
+        <v>35</v>
+      </c>
+      <c r="E1137">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="F1137" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1138">
+        <v>20250530</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1138" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1138">
+        <v>36</v>
+      </c>
+      <c r="E1138">
+        <v>7.03</v>
+      </c>
+      <c r="F1138" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1139">
+        <v>20250530</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1139" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1139">
+        <v>37</v>
+      </c>
+      <c r="E1139">
+        <v>12.86</v>
+      </c>
+      <c r="F1139" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1140">
+        <v>20250530</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1140" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1140">
+        <v>38</v>
+      </c>
+      <c r="E1140">
+        <v>10.45</v>
+      </c>
+      <c r="F1140" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1141">
+        <v>20250530</v>
+      </c>
+      <c r="B1141" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1141" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1141">
+        <v>39</v>
+      </c>
+      <c r="E1141">
+        <v>10.85</v>
+      </c>
+      <c r="F1141" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1142">
+        <v>20250530</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1142" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1142">
+        <v>40</v>
+      </c>
+      <c r="E1142">
+        <v>10.71</v>
+      </c>
+      <c r="F1142" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1143">
+        <v>20250530</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1143" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1143">
+        <v>41</v>
+      </c>
+      <c r="E1143">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="F1143" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1144">
+        <v>20250530</v>
+      </c>
+      <c r="B1144" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1144" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1144">
+        <v>42</v>
+      </c>
+      <c r="E1144">
+        <v>9.66</v>
+      </c>
+      <c r="F1144" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1145">
+        <v>20250530</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1145" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1145">
+        <v>43</v>
+      </c>
+      <c r="E1145">
+        <v>13.66</v>
+      </c>
+      <c r="F1145" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1146">
+        <v>20250530</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1146" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1146">
+        <v>44</v>
+      </c>
+      <c r="E1146">
+        <v>8.1</v>
+      </c>
+      <c r="F1146" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1147">
+        <v>20250530</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1147" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1147">
+        <v>45</v>
+      </c>
+      <c r="E1147">
+        <v>9.4</v>
+      </c>
+      <c r="F1147" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1148">
+        <v>20250530</v>
+      </c>
+      <c r="B1148" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1148" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1148">
+        <v>46</v>
+      </c>
+      <c r="E1148">
+        <v>7.74</v>
+      </c>
+      <c r="F1148" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1149">
+        <v>20250530</v>
+      </c>
+      <c r="B1149" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1149" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1149">
+        <v>47</v>
+      </c>
+      <c r="E1149">
+        <v>11.01</v>
+      </c>
+      <c r="F1149" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1150">
+        <v>20250530</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1150" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1150">
+        <v>48</v>
+      </c>
+      <c r="E1150">
+        <v>12.89</v>
+      </c>
+      <c r="F1150" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1151">
+        <v>20250530</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1151" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1151">
+        <v>49</v>
+      </c>
+      <c r="E1151">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F1151" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1152">
+        <v>20250530</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1152" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1152">
+        <v>50</v>
+      </c>
+      <c r="E1152">
+        <v>9.42</v>
+      </c>
+      <c r="F1152" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1153">
+        <v>20250530</v>
+      </c>
+      <c r="B1153" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1153" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1153">
+        <v>51</v>
+      </c>
+      <c r="E1153">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="F1153" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1154">
+        <v>20250530</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1154">
+        <v>52</v>
+      </c>
+      <c r="E1154">
+        <v>10</v>
+      </c>
+      <c r="F1154" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1155">
+        <v>20250530</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1155">
+        <v>53</v>
+      </c>
+      <c r="E1155">
+        <v>11.62</v>
+      </c>
+      <c r="F1155" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1156">
+        <v>20250530</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1156" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1156">
+        <v>54</v>
+      </c>
+      <c r="E1156">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="F1156" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1157">
+        <v>20250530</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1157" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1157">
+        <v>55</v>
+      </c>
+      <c r="E1157">
+        <v>12.49</v>
+      </c>
+      <c r="F1157" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1158">
+        <v>20250530</v>
+      </c>
+      <c r="B1158" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1158" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1158">
+        <v>56</v>
+      </c>
+      <c r="E1158">
+        <v>12.26</v>
+      </c>
+      <c r="F1158" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1159">
+        <v>20250530</v>
+      </c>
+      <c r="B1159" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1159" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1159">
+        <v>57</v>
+      </c>
+      <c r="E1159">
+        <v>10.71</v>
+      </c>
+      <c r="F1159" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1160">
+        <v>20250530</v>
+      </c>
+      <c r="B1160" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1160" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1160">
+        <v>58</v>
+      </c>
+      <c r="E1160">
+        <v>8.42</v>
+      </c>
+      <c r="F1160" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1161">
+        <v>20250530</v>
+      </c>
+      <c r="B1161" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1161" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1161">
+        <v>59</v>
+      </c>
+      <c r="E1161">
+        <v>8.49</v>
+      </c>
+      <c r="F1161" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1162">
+        <v>20250530</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1162">
+        <v>60</v>
+      </c>
+      <c r="E1162">
+        <v>9.27</v>
+      </c>
+      <c r="F1162" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1163">
+        <v>20250530</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1163">
+        <v>61</v>
+      </c>
+      <c r="E1163">
+        <v>8.58</v>
+      </c>
+      <c r="F1163" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1164">
+        <v>20250530</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1164" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1164">
+        <v>62</v>
+      </c>
+      <c r="E1164">
+        <v>11.63</v>
+      </c>
+      <c r="F1164" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1165">
+        <v>20250530</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1165" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1165">
+        <v>63</v>
+      </c>
+      <c r="E1165">
+        <v>10</v>
+      </c>
+      <c r="F1165" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1166">
+        <v>20250530</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1166" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1166">
+        <v>64</v>
+      </c>
+      <c r="E1166">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="F1166" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1167">
+        <v>20250530</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1167">
+        <v>65</v>
+      </c>
+      <c r="E1167">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="F1167" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1168">
+        <v>20250530</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1168">
+        <v>66</v>
+      </c>
+      <c r="E1168">
+        <v>9.82</v>
+      </c>
+      <c r="F1168" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1169">
+        <v>20250530</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1169" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1169">
+        <v>67</v>
+      </c>
+      <c r="E1169">
+        <v>8.74</v>
+      </c>
+      <c r="F1169" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1170">
+        <v>20250530</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1170">
+        <v>68</v>
+      </c>
+      <c r="E1170">
+        <v>9.15</v>
+      </c>
+      <c r="F1170" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1171">
+        <v>20250530</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1171">
+        <v>69</v>
+      </c>
+      <c r="E1171">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="F1171" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1172">
+        <v>20250530</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1172">
+        <v>70</v>
+      </c>
+      <c r="E1172">
+        <v>11.3</v>
+      </c>
+      <c r="F1172" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1173">
+        <v>20250530</v>
+      </c>
+      <c r="B1173" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1173" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1173">
+        <v>71</v>
+      </c>
+      <c r="E1173">
+        <v>10.82</v>
+      </c>
+      <c r="F1173" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1174">
+        <v>20250530</v>
+      </c>
+      <c r="B1174" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1174" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1174">
+        <v>72</v>
+      </c>
+      <c r="E1174">
+        <v>6.66</v>
+      </c>
+      <c r="F1174" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1175">
+        <v>20250530</v>
+      </c>
+      <c r="B1175" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1175" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1175">
+        <v>73</v>
+      </c>
+      <c r="E1175">
+        <v>6.66</v>
+      </c>
+      <c r="F1175" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1176">
+        <v>20250530</v>
+      </c>
+      <c r="B1176" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1176" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1176">
+        <v>74</v>
+      </c>
+      <c r="E1176">
+        <v>8.9</v>
+      </c>
+      <c r="F1176" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1177">
+        <v>20250530</v>
+      </c>
+      <c r="B1177" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1177" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1177">
+        <v>75</v>
+      </c>
+      <c r="E1177">
+        <v>10.52</v>
+      </c>
+      <c r="F1177" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1178">
+        <v>20250530</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1178" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1178">
+        <v>76</v>
+      </c>
+      <c r="E1178">
+        <v>10.17</v>
+      </c>
+      <c r="F1178" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1179">
+        <v>20250530</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1179" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1179">
+        <v>77</v>
+      </c>
+      <c r="E1179">
+        <v>12.74</v>
+      </c>
+      <c r="F1179" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1180">
+        <v>20250530</v>
+      </c>
+      <c r="B1180" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1180" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1180">
+        <v>78</v>
+      </c>
+      <c r="E1180">
+        <v>9.31</v>
+      </c>
+      <c r="F1180" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1181">
+        <v>20250530</v>
+      </c>
+      <c r="B1181" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1181" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1181">
+        <v>79</v>
+      </c>
+      <c r="E1181">
+        <v>9.1</v>
+      </c>
+      <c r="F1181" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1182">
+        <v>20250530</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1182" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1182">
+        <v>80</v>
+      </c>
+      <c r="E1182">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="F1182" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1183">
+        <v>20250530</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1183" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1183">
+        <v>81</v>
+      </c>
+      <c r="E1183">
+        <v>7.57</v>
+      </c>
+      <c r="F1183" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1184">
+        <v>20250530</v>
+      </c>
+      <c r="B1184" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1184" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1184">
+        <v>82</v>
+      </c>
+      <c r="E1184">
+        <v>10.17</v>
+      </c>
+      <c r="F1184" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1185">
+        <v>20250530</v>
+      </c>
+      <c r="B1185" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1185" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1185">
+        <v>83</v>
+      </c>
+      <c r="E1185">
+        <v>13.64</v>
+      </c>
+      <c r="F1185" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1186">
+        <v>20250530</v>
+      </c>
+      <c r="B1186" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1186" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1186">
+        <v>84</v>
+      </c>
+      <c r="E1186">
+        <v>11.67</v>
+      </c>
+      <c r="F1186" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1187">
+        <v>20250530</v>
+      </c>
+      <c r="B1187" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1187" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1187">
+        <v>85</v>
+      </c>
+      <c r="E1187">
+        <v>8.49</v>
+      </c>
+      <c r="F1187" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1188">
+        <v>20250530</v>
+      </c>
+      <c r="B1188" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1188" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1188">
+        <v>86</v>
+      </c>
+      <c r="E1188">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="F1188" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1189">
+        <v>20250530</v>
+      </c>
+      <c r="B1189" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1189" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1189">
+        <v>87</v>
+      </c>
+      <c r="E1189">
+        <v>11.1</v>
+      </c>
+      <c r="F1189" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1190">
+        <v>20250530</v>
+      </c>
+      <c r="B1190" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1190" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1190">
+        <v>88</v>
+      </c>
+      <c r="E1190">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="F1190" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1191">
+        <v>20250530</v>
+      </c>
+      <c r="B1191" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1191" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1191">
+        <v>89</v>
+      </c>
+      <c r="E1191">
+        <v>10.07</v>
+      </c>
+      <c r="F1191" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1192">
+        <v>20250530</v>
+      </c>
+      <c r="B1192" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1192" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1192">
+        <v>90</v>
+      </c>
+      <c r="E1192">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="F1192" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1193">
+        <v>20250530</v>
+      </c>
+      <c r="B1193" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1193" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1193">
+        <v>91</v>
+      </c>
+      <c r="E1193">
+        <v>6.94</v>
+      </c>
+      <c r="F1193" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1194">
+        <v>20250530</v>
+      </c>
+      <c r="B1194" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1194" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1194">
+        <v>92</v>
+      </c>
+      <c r="E1194">
+        <v>11.8</v>
+      </c>
+      <c r="F1194" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1195">
+        <v>20250530</v>
+      </c>
+      <c r="B1195" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1195" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1195">
+        <v>93</v>
+      </c>
+      <c r="E1195">
+        <v>10.53</v>
+      </c>
+      <c r="F1195" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1196">
+        <v>20250530</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1196" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1196">
+        <v>94</v>
+      </c>
+      <c r="E1196">
+        <v>11.37</v>
+      </c>
+      <c r="F1196" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1197">
+        <v>20250530</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1197" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1197">
+        <v>95</v>
+      </c>
+      <c r="E1197">
+        <v>12.61</v>
+      </c>
+      <c r="F1197" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1198">
+        <v>20250530</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1198" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1198">
+        <v>96</v>
+      </c>
+      <c r="E1198">
+        <v>11.79</v>
+      </c>
+      <c r="F1198" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1199">
+        <v>20250530</v>
+      </c>
+      <c r="B1199" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1199" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1199">
+        <v>97</v>
+      </c>
+      <c r="E1199">
+        <v>9.33</v>
+      </c>
+      <c r="F1199" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1200">
+        <v>20250530</v>
+      </c>
+      <c r="B1200" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1200" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1200">
+        <v>98</v>
+      </c>
+      <c r="E1200">
+        <v>9.83</v>
+      </c>
+      <c r="F1200" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1201">
+        <v>20250530</v>
+      </c>
+      <c r="B1201" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1201" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1201">
+        <v>99</v>
+      </c>
+      <c r="E1201">
+        <v>8.65</v>
+      </c>
+      <c r="F1201" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1202">
+        <v>20250530</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1202" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1202">
+        <v>100</v>
+      </c>
+      <c r="E1202">
+        <v>10.44</v>
+      </c>
+      <c r="F1202" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>